<commit_message>
fix hungarian 3 - missing keys in destribution keys - Dimo helped
</commit_message>
<xml_diff>
--- a/DimoPdfToExcelSln/DimoPdfToExcelWeb/wwwroot/Files/HungarianDistributionKeys.xlsx
+++ b/DimoPdfToExcelSln/DimoPdfToExcelWeb/wwwroot/Files/HungarianDistributionKeys.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimo.statkov\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\corewebtest\DimoPdfToExcelSln\DimoPdfToExcelWeb\wwwroot\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="225">
   <si>
     <t>G. Accrued &amp; Deffered Expenses</t>
   </si>
@@ -691,6 +691,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Rendkívüli bevételek</t>
+  </si>
+  <si>
+    <t>000. 00. Rendkívüli ráfordítások</t>
+  </si>
+  <si>
+    <t>Extraordinary expenses</t>
   </si>
 </sst>
 </file>
@@ -799,7 +808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -823,6 +832,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1105,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,6 +1161,9 @@
         <v>29</v>
       </c>
       <c r="B4" s="2"/>
+      <c r="C4" s="15">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1231,6 +1247,9 @@
         <v>40</v>
       </c>
       <c r="B12" s="2"/>
+      <c r="C12" s="15">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1314,6 +1333,9 @@
         <v>41</v>
       </c>
       <c r="B20" s="2"/>
+      <c r="C20" s="15">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1436,6 +1458,9 @@
         <v>66</v>
       </c>
       <c r="B32" s="2"/>
+      <c r="C32" s="15">
+        <v>28</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
@@ -1508,6 +1533,9 @@
         <v>77</v>
       </c>
       <c r="B39" s="2"/>
+      <c r="C39" s="15">
+        <v>33</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
@@ -1602,6 +1630,9 @@
         <v>90</v>
       </c>
       <c r="B48" s="2"/>
+      <c r="C48" s="15">
+        <v>39</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
@@ -1674,6 +1705,9 @@
         <v>99</v>
       </c>
       <c r="B55" s="2"/>
+      <c r="C55" s="15">
+        <v>41</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
@@ -1702,6 +1736,9 @@
         <v>102</v>
       </c>
       <c r="B58" s="2"/>
+      <c r="C58" s="15">
+        <v>43</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
@@ -1858,6 +1895,9 @@
         <v>124</v>
       </c>
       <c r="B76" s="6"/>
+      <c r="C76" s="15">
+        <v>64</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
@@ -1903,6 +1943,9 @@
         <v>132</v>
       </c>
       <c r="B81" s="2"/>
+      <c r="C81" s="15">
+        <v>76</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
@@ -1953,6 +1996,9 @@
         <v>137</v>
       </c>
       <c r="B86" s="2"/>
+      <c r="C86" s="15">
+        <v>76</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
@@ -2058,6 +2104,9 @@
         <v>150</v>
       </c>
       <c r="B96" s="2"/>
+      <c r="C96" s="15">
+        <v>81</v>
+      </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
@@ -2191,6 +2240,9 @@
         <v>165</v>
       </c>
       <c r="B109" s="2"/>
+      <c r="C109" s="15">
+        <v>89</v>
+      </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
@@ -2239,10 +2291,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D49"/>
+  <dimension ref="A2:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2293,6 +2345,9 @@
         <v>174</v>
       </c>
       <c r="B5" s="2"/>
+      <c r="C5" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -2321,6 +2376,9 @@
         <v>177</v>
       </c>
       <c r="B8" s="2"/>
+      <c r="C8" s="15">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -2414,6 +2472,12 @@
         <v>185</v>
       </c>
       <c r="B16" s="2"/>
+      <c r="C16" s="15">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -2462,6 +2526,12 @@
         <v>189</v>
       </c>
       <c r="B20" s="2"/>
+      <c r="C20" s="15">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -2621,6 +2691,9 @@
         <v>205</v>
       </c>
       <c r="B35" s="2"/>
+      <c r="C35" s="15">
+        <v>66</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
@@ -2729,6 +2802,12 @@
         <v>213</v>
       </c>
       <c r="B45" s="2"/>
+      <c r="C45" s="15">
+        <v>78</v>
+      </c>
+      <c r="D45" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -2756,11 +2835,34 @@
         <v>221</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>217</v>
       </c>
       <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="C51" s="18">
+        <v>88</v>
+      </c>
+      <c r="D51" t="s">
+        <v>221</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix all bs hung
</commit_message>
<xml_diff>
--- a/DimoPdfToExcelSln/DimoPdfToExcelWeb/wwwroot/Files/HungarianDistributionKeys.xlsx
+++ b/DimoPdfToExcelSln/DimoPdfToExcelWeb/wwwroot/Files/HungarianDistributionKeys.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hungarian BS" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="256">
   <si>
     <t>G. Accrued &amp; Deffered Expenses</t>
   </si>
@@ -669,9 +669,6 @@
     <t>045. C. Adózás előtti eredmény</t>
   </si>
   <si>
-    <t>046. X. Adófizetési kötelezettség</t>
-  </si>
-  <si>
     <t>047. D. Adózott eredmény</t>
   </si>
   <si>
@@ -769,6 +766,33 @@
   </si>
   <si>
     <t>Rövid lejáratú kötelezettségek</t>
+  </si>
+  <si>
+    <t>Üzemi (üzleti) tevékenység eredménye</t>
+  </si>
+  <si>
+    <t>Értékesítés nettó árbevétele</t>
+  </si>
+  <si>
+    <t>Aktivált saját teljesítmények értéke</t>
+  </si>
+  <si>
+    <t>Anyagjellegű ráfordítások</t>
+  </si>
+  <si>
+    <t>Pénzügyi műveletek bevételei</t>
+  </si>
+  <si>
+    <t>Pénzügyi műveletek ráfordításai</t>
+  </si>
+  <si>
+    <t>Pénzügyi műveletek eredménye</t>
+  </si>
+  <si>
+    <t>Adózott eredmény</t>
+  </si>
+  <si>
+    <t>046. XII. Adófizetési kötelezettség</t>
   </si>
 </sst>
 </file>
@@ -1185,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,16 +1231,16 @@
         <v>30</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>218</v>
-      </c>
       <c r="E1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>226</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1231,7 +1255,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="E3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1245,7 +1269,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1259,10 +1283,10 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F5" t="s">
         <v>228</v>
-      </c>
-      <c r="F5" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1276,10 +1300,10 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F6" t="s">
         <v>228</v>
-      </c>
-      <c r="F6" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1293,10 +1317,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F7" t="s">
         <v>228</v>
-      </c>
-      <c r="F7" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1310,10 +1334,10 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
+        <v>227</v>
+      </c>
+      <c r="F8" t="s">
         <v>228</v>
-      </c>
-      <c r="F8" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1327,10 +1351,10 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
+        <v>227</v>
+      </c>
+      <c r="F9" t="s">
         <v>228</v>
-      </c>
-      <c r="F9" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1344,10 +1368,10 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" t="s">
         <v>228</v>
-      </c>
-      <c r="F10" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1361,10 +1385,10 @@
         <v>12</v>
       </c>
       <c r="E11" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" t="s">
         <v>228</v>
-      </c>
-      <c r="F11" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1378,7 +1402,7 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1392,10 +1416,10 @@
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1409,10 +1433,10 @@
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1426,10 +1450,10 @@
         <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1443,10 +1467,10 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1460,10 +1484,10 @@
         <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1477,10 +1501,10 @@
         <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1494,10 +1518,10 @@
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1511,7 +1535,7 @@
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1525,10 +1549,10 @@
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1542,10 +1566,10 @@
         <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1559,10 +1583,10 @@
         <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1576,10 +1600,10 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1593,10 +1617,10 @@
         <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1610,10 +1634,10 @@
         <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1627,10 +1651,10 @@
         <v>23</v>
       </c>
       <c r="E27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1644,10 +1668,10 @@
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1661,10 +1685,10 @@
         <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F29" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1678,10 +1702,10 @@
         <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1701,7 +1725,7 @@
         <v>28</v>
       </c>
       <c r="E32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1715,10 +1739,10 @@
         <v>27</v>
       </c>
       <c r="E33" t="s">
+        <v>232</v>
+      </c>
+      <c r="F33" t="s">
         <v>233</v>
-      </c>
-      <c r="F33" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1732,10 +1756,10 @@
         <v>29</v>
       </c>
       <c r="E34" t="s">
+        <v>232</v>
+      </c>
+      <c r="F34" t="s">
         <v>233</v>
-      </c>
-      <c r="F34" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1749,10 +1773,10 @@
         <v>29</v>
       </c>
       <c r="E35" t="s">
+        <v>232</v>
+      </c>
+      <c r="F35" t="s">
         <v>233</v>
-      </c>
-      <c r="F35" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1766,10 +1790,10 @@
         <v>28</v>
       </c>
       <c r="E36" t="s">
+        <v>232</v>
+      </c>
+      <c r="F36" t="s">
         <v>233</v>
-      </c>
-      <c r="F36" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1783,10 +1807,10 @@
         <v>28</v>
       </c>
       <c r="E37" t="s">
+        <v>232</v>
+      </c>
+      <c r="F37" t="s">
         <v>233</v>
-      </c>
-      <c r="F37" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1800,10 +1824,10 @@
         <v>30</v>
       </c>
       <c r="E38" t="s">
+        <v>232</v>
+      </c>
+      <c r="F38" t="s">
         <v>233</v>
-      </c>
-      <c r="F38" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1815,7 +1839,7 @@
         <v>33</v>
       </c>
       <c r="E39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1829,10 +1853,10 @@
         <v>33</v>
       </c>
       <c r="E40" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F40" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1846,10 +1870,10 @@
         <v>35</v>
       </c>
       <c r="E41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1863,10 +1887,10 @@
         <v>35</v>
       </c>
       <c r="E42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1880,10 +1904,10 @@
         <v>35</v>
       </c>
       <c r="E43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1897,10 +1921,10 @@
         <v>37</v>
       </c>
       <c r="E44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1914,10 +1938,10 @@
         <v>37</v>
       </c>
       <c r="E45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1931,10 +1955,10 @@
         <v>37</v>
       </c>
       <c r="E46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1948,10 +1972,10 @@
         <v>37</v>
       </c>
       <c r="E47" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F47" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1963,7 +1987,7 @@
         <v>39</v>
       </c>
       <c r="E48" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1977,10 +2001,10 @@
         <v>39</v>
       </c>
       <c r="E49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1994,10 +2018,10 @@
         <v>39</v>
       </c>
       <c r="E50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F50" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2011,10 +2035,10 @@
         <v>39</v>
       </c>
       <c r="E51" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F51" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2028,10 +2052,10 @@
         <v>39</v>
       </c>
       <c r="E52" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F52" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2045,10 +2069,10 @@
         <v>39</v>
       </c>
       <c r="E53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F53" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2062,10 +2086,10 @@
         <v>39</v>
       </c>
       <c r="E54" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F54" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2077,7 +2101,7 @@
         <v>41</v>
       </c>
       <c r="E55" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2091,10 +2115,10 @@
         <v>41</v>
       </c>
       <c r="E56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F56" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2108,10 +2132,10 @@
         <v>41</v>
       </c>
       <c r="E57" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2134,7 +2158,7 @@
         <v>43</v>
       </c>
       <c r="E59" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2148,7 +2172,7 @@
         <v>43</v>
       </c>
       <c r="E60" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2162,7 +2186,7 @@
         <v>43</v>
       </c>
       <c r="E61" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2198,7 +2222,7 @@
         <v>48</v>
       </c>
       <c r="E66" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2207,10 +2231,10 @@
       </c>
       <c r="B67" s="4"/>
       <c r="E67" t="s">
+        <v>238</v>
+      </c>
+      <c r="F67" t="s">
         <v>239</v>
-      </c>
-      <c r="F67" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2224,7 +2248,7 @@
         <v>48</v>
       </c>
       <c r="E68" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2238,7 +2262,7 @@
         <v>50</v>
       </c>
       <c r="E69" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2252,7 +2276,7 @@
         <v>52</v>
       </c>
       <c r="E70" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2266,7 +2290,7 @@
         <v>51</v>
       </c>
       <c r="E71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2280,7 +2304,7 @@
         <v>51</v>
       </c>
       <c r="E72" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2289,10 +2313,10 @@
       </c>
       <c r="B73" s="4"/>
       <c r="E73" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F73" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2301,10 +2325,10 @@
       </c>
       <c r="B74" s="4"/>
       <c r="E74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F74" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2318,7 +2342,7 @@
         <v>52</v>
       </c>
       <c r="E75" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2341,7 +2365,7 @@
         <v>64</v>
       </c>
       <c r="E77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2355,7 +2379,7 @@
         <v>64</v>
       </c>
       <c r="E78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2369,7 +2393,7 @@
         <v>64</v>
       </c>
       <c r="E79" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2389,7 +2413,7 @@
         <v>76</v>
       </c>
       <c r="E81" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2403,10 +2427,10 @@
         <v>73</v>
       </c>
       <c r="E82" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F82" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2420,10 +2444,10 @@
         <v>73</v>
       </c>
       <c r="E83" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F83" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2437,10 +2461,10 @@
         <v>76</v>
       </c>
       <c r="E84" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F84" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2454,10 +2478,10 @@
         <v>76</v>
       </c>
       <c r="E85" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F85" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2469,7 +2493,7 @@
         <v>76</v>
       </c>
       <c r="E86" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2483,10 +2507,10 @@
         <v>68</v>
       </c>
       <c r="E87" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F87" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2500,10 +2524,10 @@
         <v>69</v>
       </c>
       <c r="E88" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F88" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2517,10 +2541,10 @@
         <v>69</v>
       </c>
       <c r="E89" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F89" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2534,10 +2558,10 @@
         <v>68</v>
       </c>
       <c r="E90" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F90" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2551,10 +2575,10 @@
         <v>76</v>
       </c>
       <c r="E91" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F91" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2568,10 +2592,10 @@
         <v>72</v>
       </c>
       <c r="E92" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F92" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2585,10 +2609,10 @@
         <v>72</v>
       </c>
       <c r="E93" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F93" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2602,10 +2626,10 @@
         <v>76</v>
       </c>
       <c r="E94" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F94" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2619,10 +2643,10 @@
         <v>76</v>
       </c>
       <c r="E95" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F95" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2636,12 +2660,12 @@
         <v>81</v>
       </c>
       <c r="E96" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>149</v>
@@ -2650,10 +2674,10 @@
         <v>68</v>
       </c>
       <c r="E97" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F97" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2662,10 +2686,10 @@
       </c>
       <c r="B98" s="4"/>
       <c r="E98" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F98" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2679,10 +2703,10 @@
         <v>68</v>
       </c>
       <c r="E99" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F99" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2696,10 +2720,10 @@
         <v>80</v>
       </c>
       <c r="E100" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F100" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2713,10 +2737,10 @@
         <v>81</v>
       </c>
       <c r="E101" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F101" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2730,10 +2754,10 @@
         <v>87</v>
       </c>
       <c r="E102" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F102" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2747,10 +2771,10 @@
         <v>83</v>
       </c>
       <c r="E103" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F103" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2764,10 +2788,10 @@
         <v>83</v>
       </c>
       <c r="E104" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F104" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -2781,10 +2805,10 @@
         <v>87</v>
       </c>
       <c r="E105" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F105" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -2798,10 +2822,10 @@
         <v>87</v>
       </c>
       <c r="E106" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F106" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -2815,10 +2839,10 @@
         <v>87</v>
       </c>
       <c r="E107" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F107" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -2832,10 +2856,10 @@
         <v>87</v>
       </c>
       <c r="E108" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F108" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -2860,7 +2884,7 @@
         <v>89</v>
       </c>
       <c r="E110" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -2874,7 +2898,7 @@
         <v>89</v>
       </c>
       <c r="E111" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -2888,7 +2912,7 @@
         <v>89</v>
       </c>
       <c r="E112" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2905,9 +2929,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D51"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
@@ -2916,56 +2940,96 @@
     <col min="1" max="1" width="95.28515625" customWidth="1"/>
     <col min="2" max="2" width="46.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="48" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="15">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>247</v>
+      </c>
+      <c r="F5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>20</v>
@@ -2973,129 +3037,186 @@
       <c r="C6">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7">
+      <c r="E6" t="s">
+        <v>247</v>
+      </c>
+      <c r="F6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="15">
+      <c r="E7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="E9" t="s">
+        <v>247</v>
+      </c>
+      <c r="F9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" t="s">
+        <v>247</v>
+      </c>
+      <c r="F10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>218</v>
+      </c>
+      <c r="E12" t="s">
+        <v>247</v>
+      </c>
+      <c r="F12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>218</v>
+      </c>
+      <c r="E13" t="s">
+        <v>247</v>
+      </c>
+      <c r="F13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>218</v>
+      </c>
+      <c r="E14" t="s">
+        <v>247</v>
+      </c>
+      <c r="F14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="15">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>218</v>
+      </c>
+      <c r="E15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="15">
-        <v>24</v>
+      <c r="C16">
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="E16" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>16</v>
@@ -3104,12 +3225,15 @@
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="E17" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>16</v>
@@ -3118,272 +3242,395 @@
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B19" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="15">
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="15">
-        <v>30</v>
+        <v>218</v>
+      </c>
+      <c r="E19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="E20" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="E21" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>15</v>
+        <v>190</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C22">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23">
-        <v>44</v>
-      </c>
-      <c r="D23" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E22" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
+        <v>253</v>
+      </c>
+      <c r="F24" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B25" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>54</v>
+      </c>
+      <c r="E25" t="s">
+        <v>253</v>
+      </c>
+      <c r="F25" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B26" s="12" t="s">
+      <c r="E26" t="s">
+        <v>253</v>
+      </c>
+      <c r="F26" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>253</v>
+      </c>
+      <c r="F27" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B28" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>56</v>
+      </c>
+      <c r="E28" t="s">
+        <v>253</v>
+      </c>
+      <c r="F28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C28">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>11</v>
-      </c>
       <c r="C29">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="E29" t="s">
+        <v>253</v>
+      </c>
+      <c r="F29" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B30" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>60</v>
+      </c>
+      <c r="E30" t="s">
+        <v>253</v>
+      </c>
+      <c r="F30" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C30">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="C31">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
+        <v>253</v>
+      </c>
+      <c r="F31" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>9</v>
+        <v>201</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C32">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="E32" t="s">
+        <v>253</v>
+      </c>
+      <c r="F32" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B33" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="E33" t="s">
+        <v>253</v>
+      </c>
+      <c r="F33" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C33">
+      <c r="C34" s="15">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="15">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>253</v>
+      </c>
+      <c r="F34" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35">
+        <v>70</v>
+      </c>
+      <c r="D35" t="s">
+        <v>218</v>
+      </c>
+      <c r="E35" t="s">
+        <v>253</v>
+      </c>
+      <c r="F35" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36">
-        <v>70</v>
-      </c>
-      <c r="D36" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="E36" t="s">
+        <v>253</v>
+      </c>
+      <c r="F36" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>76</v>
+      </c>
+      <c r="D37" t="s">
+        <v>218</v>
+      </c>
+      <c r="E37" t="s">
+        <v>253</v>
+      </c>
+      <c r="F37" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38">
-        <v>76</v>
-      </c>
-      <c r="D38" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="E38" t="s">
+        <v>253</v>
+      </c>
+      <c r="F38" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s">
+        <v>218</v>
+      </c>
+      <c r="E39" t="s">
+        <v>253</v>
+      </c>
+      <c r="F39" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D40" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="E40" t="s">
+        <v>253</v>
+      </c>
+      <c r="F40" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C41">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D41" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="E41" t="s">
+        <v>253</v>
+      </c>
+      <c r="F41" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>3</v>
@@ -3392,99 +3639,103 @@
         <v>78</v>
       </c>
       <c r="D42" t="s">
+        <v>218</v>
+      </c>
+      <c r="E42" t="s">
+        <v>253</v>
+      </c>
+      <c r="F42" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="E43" t="s">
+        <v>253</v>
+      </c>
+      <c r="F43" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="15">
+        <v>78</v>
+      </c>
+      <c r="D44" t="s">
+        <v>218</v>
+      </c>
+      <c r="E44" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C47" s="15">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="B48" s="15" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43">
-        <v>78</v>
-      </c>
-      <c r="D43" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="15">
-        <v>78</v>
-      </c>
-      <c r="D45" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="C48" s="15">
+        <v>88</v>
+      </c>
+      <c r="D48" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>92</v>
+      </c>
+      <c r="D49" t="s">
+        <v>218</v>
+      </c>
+      <c r="E49" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C48">
-        <v>92</v>
-      </c>
-      <c r="D48" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="C50" s="15">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="C51" s="15">
-        <v>88</v>
-      </c>
-      <c r="D51" t="s">
-        <v>219</v>
-      </c>
+      <c r="B50" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bih changes. Fix all hungarian including Hungarian9
</commit_message>
<xml_diff>
--- a/DimoPdfToExcelSln/DimoPdfToExcelWeb/wwwroot/Files/HungarianDistributionKeys.xlsx
+++ b/DimoPdfToExcelSln/DimoPdfToExcelWeb/wwwroot/Files/HungarianDistributionKeys.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="259">
   <si>
     <t>G. Accrued &amp; Deffered Expenses</t>
   </si>
@@ -489,9 +489,6 @@
     <t>Advances from customers</t>
   </si>
   <si>
-    <t>099. 4. Kötelezettségek áruszállításból és</t>
-  </si>
-  <si>
     <t>Liabilities from trade &amp; services</t>
   </si>
   <si>
@@ -799,6 +796,12 @@
   </si>
   <si>
     <t>Yordan44</t>
+  </si>
+  <si>
+    <t>099. 4. Kötelezettségek áruszállításból és szolgáltatásból (szállítók)</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -1215,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,22 +1234,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>217</v>
-      </c>
       <c r="E1" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>225</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1261,7 +1264,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="E3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1275,7 +1278,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1289,10 +1292,10 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F5" t="s">
         <v>227</v>
-      </c>
-      <c r="F5" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1306,10 +1309,10 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F6" t="s">
         <v>227</v>
-      </c>
-      <c r="F6" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1323,10 +1326,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
+        <v>226</v>
+      </c>
+      <c r="F7" t="s">
         <v>227</v>
-      </c>
-      <c r="F7" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1340,10 +1343,10 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
+        <v>226</v>
+      </c>
+      <c r="F8" t="s">
         <v>227</v>
-      </c>
-      <c r="F8" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1357,10 +1360,10 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
+        <v>226</v>
+      </c>
+      <c r="F9" t="s">
         <v>227</v>
-      </c>
-      <c r="F9" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1374,10 +1377,10 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
+        <v>226</v>
+      </c>
+      <c r="F10" t="s">
         <v>227</v>
-      </c>
-      <c r="F10" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1391,10 +1394,10 @@
         <v>12</v>
       </c>
       <c r="E11" t="s">
+        <v>226</v>
+      </c>
+      <c r="F11" t="s">
         <v>227</v>
-      </c>
-      <c r="F11" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1408,7 +1411,7 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1422,10 +1425,10 @@
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1439,10 +1442,10 @@
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1456,10 +1459,10 @@
         <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1473,10 +1476,10 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1490,10 +1493,10 @@
         <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1507,10 +1510,10 @@
         <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1524,10 +1527,10 @@
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1541,7 +1544,7 @@
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1555,10 +1558,10 @@
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,10 +1575,10 @@
         <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1589,10 +1592,10 @@
         <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1606,10 +1609,10 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1623,10 +1626,10 @@
         <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1640,10 +1643,10 @@
         <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1657,10 +1660,10 @@
         <v>23</v>
       </c>
       <c r="E27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1674,10 +1677,10 @@
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1691,10 +1694,10 @@
         <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1708,10 +1711,10 @@
         <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1731,7 +1734,7 @@
         <v>28</v>
       </c>
       <c r="E32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1745,10 +1748,10 @@
         <v>27</v>
       </c>
       <c r="E33" t="s">
+        <v>231</v>
+      </c>
+      <c r="F33" t="s">
         <v>232</v>
-      </c>
-      <c r="F33" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1762,10 +1765,10 @@
         <v>29</v>
       </c>
       <c r="E34" t="s">
+        <v>231</v>
+      </c>
+      <c r="F34" t="s">
         <v>232</v>
-      </c>
-      <c r="F34" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1779,10 +1782,10 @@
         <v>29</v>
       </c>
       <c r="E35" t="s">
+        <v>231</v>
+      </c>
+      <c r="F35" t="s">
         <v>232</v>
-      </c>
-      <c r="F35" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1796,10 +1799,10 @@
         <v>28</v>
       </c>
       <c r="E36" t="s">
+        <v>231</v>
+      </c>
+      <c r="F36" t="s">
         <v>232</v>
-      </c>
-      <c r="F36" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1813,10 +1816,10 @@
         <v>28</v>
       </c>
       <c r="E37" t="s">
+        <v>231</v>
+      </c>
+      <c r="F37" t="s">
         <v>232</v>
-      </c>
-      <c r="F37" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1830,10 +1833,10 @@
         <v>30</v>
       </c>
       <c r="E38" t="s">
+        <v>231</v>
+      </c>
+      <c r="F38" t="s">
         <v>232</v>
-      </c>
-      <c r="F38" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1845,7 +1848,7 @@
         <v>33</v>
       </c>
       <c r="E39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1859,10 +1862,10 @@
         <v>33</v>
       </c>
       <c r="E40" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F40" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1876,10 +1879,10 @@
         <v>35</v>
       </c>
       <c r="E41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1893,10 +1896,10 @@
         <v>35</v>
       </c>
       <c r="E42" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1910,10 +1913,10 @@
         <v>35</v>
       </c>
       <c r="E43" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1927,10 +1930,10 @@
         <v>37</v>
       </c>
       <c r="E44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1944,10 +1947,10 @@
         <v>37</v>
       </c>
       <c r="E45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1961,10 +1964,10 @@
         <v>37</v>
       </c>
       <c r="E46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1978,10 +1981,10 @@
         <v>37</v>
       </c>
       <c r="E47" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F47" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1993,7 +1996,7 @@
         <v>39</v>
       </c>
       <c r="E48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2007,10 +2010,10 @@
         <v>39</v>
       </c>
       <c r="E49" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F49" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2024,10 +2027,10 @@
         <v>39</v>
       </c>
       <c r="E50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2041,10 +2044,10 @@
         <v>39</v>
       </c>
       <c r="E51" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F51" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2058,10 +2061,10 @@
         <v>39</v>
       </c>
       <c r="E52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F52" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2075,10 +2078,10 @@
         <v>39</v>
       </c>
       <c r="E53" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2092,10 +2095,10 @@
         <v>39</v>
       </c>
       <c r="E54" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F54" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2107,7 +2110,7 @@
         <v>41</v>
       </c>
       <c r="E55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2121,10 +2124,10 @@
         <v>41</v>
       </c>
       <c r="E56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F56" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2138,10 +2141,10 @@
         <v>41</v>
       </c>
       <c r="E57" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F57" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2164,7 +2167,7 @@
         <v>43</v>
       </c>
       <c r="E59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2178,7 +2181,7 @@
         <v>43</v>
       </c>
       <c r="E60" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2192,7 +2195,7 @@
         <v>43</v>
       </c>
       <c r="E61" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2228,7 +2231,7 @@
         <v>48</v>
       </c>
       <c r="E66" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2237,10 +2240,10 @@
       </c>
       <c r="B67" s="4"/>
       <c r="E67" t="s">
+        <v>237</v>
+      </c>
+      <c r="F67" t="s">
         <v>238</v>
-      </c>
-      <c r="F67" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2254,7 +2257,7 @@
         <v>48</v>
       </c>
       <c r="E68" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2268,7 +2271,7 @@
         <v>50</v>
       </c>
       <c r="E69" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2282,7 +2285,7 @@
         <v>52</v>
       </c>
       <c r="E70" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2296,7 +2299,7 @@
         <v>51</v>
       </c>
       <c r="E71" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2310,7 +2313,7 @@
         <v>51</v>
       </c>
       <c r="E72" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2319,10 +2322,10 @@
       </c>
       <c r="B73" s="4"/>
       <c r="E73" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F73" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2331,10 +2334,10 @@
       </c>
       <c r="B74" s="4"/>
       <c r="E74" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F74" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2348,7 +2351,7 @@
         <v>52</v>
       </c>
       <c r="E75" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2371,7 +2374,7 @@
         <v>64</v>
       </c>
       <c r="E77" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2385,7 +2388,7 @@
         <v>64</v>
       </c>
       <c r="E78" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2399,7 +2402,7 @@
         <v>64</v>
       </c>
       <c r="E79" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2419,7 +2422,7 @@
         <v>76</v>
       </c>
       <c r="E81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2433,10 +2436,10 @@
         <v>73</v>
       </c>
       <c r="E82" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F82" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2450,10 +2453,10 @@
         <v>73</v>
       </c>
       <c r="E83" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F83" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2467,10 +2470,10 @@
         <v>76</v>
       </c>
       <c r="E84" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F84" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2484,10 +2487,10 @@
         <v>76</v>
       </c>
       <c r="E85" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F85" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2499,7 +2502,7 @@
         <v>76</v>
       </c>
       <c r="E86" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2513,10 +2516,10 @@
         <v>68</v>
       </c>
       <c r="E87" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F87" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2530,10 +2533,10 @@
         <v>69</v>
       </c>
       <c r="E88" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F88" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2547,10 +2550,10 @@
         <v>69</v>
       </c>
       <c r="E89" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F89" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2564,10 +2567,10 @@
         <v>68</v>
       </c>
       <c r="E90" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F90" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2581,10 +2584,10 @@
         <v>76</v>
       </c>
       <c r="E91" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F91" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2598,10 +2601,10 @@
         <v>72</v>
       </c>
       <c r="E92" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F92" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2615,10 +2618,10 @@
         <v>72</v>
       </c>
       <c r="E93" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F93" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2632,10 +2635,10 @@
         <v>76</v>
       </c>
       <c r="E94" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F94" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2649,10 +2652,10 @@
         <v>76</v>
       </c>
       <c r="E95" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F95" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2660,18 +2663,18 @@
         <v>148</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C96" s="15">
         <v>81</v>
       </c>
       <c r="E96" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>149</v>
@@ -2680,10 +2683,10 @@
         <v>68</v>
       </c>
       <c r="E97" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F97" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2692,10 +2695,10 @@
       </c>
       <c r="B98" s="4"/>
       <c r="E98" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F98" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2709,10 +2712,10 @@
         <v>68</v>
       </c>
       <c r="E99" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F99" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2726,49 +2729,49 @@
         <v>80</v>
       </c>
       <c r="E100" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F100" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B101" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="C101">
         <v>81</v>
       </c>
       <c r="E101" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F101" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C102">
         <v>87</v>
       </c>
       <c r="E102" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F102" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>1</v>
@@ -2777,15 +2780,15 @@
         <v>83</v>
       </c>
       <c r="E103" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F103" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>1</v>
@@ -2794,83 +2797,83 @@
         <v>83</v>
       </c>
       <c r="E104" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F104" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C105">
         <v>87</v>
       </c>
       <c r="E105" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F105" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C106">
         <v>87</v>
       </c>
       <c r="E106" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F106" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C107">
         <v>87</v>
       </c>
       <c r="E107" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F107" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C108">
         <v>87</v>
       </c>
       <c r="E108" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F108" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>0</v>
@@ -2881,7 +2884,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>0</v>
@@ -2890,12 +2893,12 @@
         <v>89</v>
       </c>
       <c r="E110" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>0</v>
@@ -2904,12 +2907,12 @@
         <v>89</v>
       </c>
       <c r="E111" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B112" s="8" t="s">
         <v>0</v>
@@ -2918,12 +2921,12 @@
         <v>89</v>
       </c>
       <c r="E112" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B113" s="2"/>
     </row>
@@ -2937,8 +2940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2952,27 +2955,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E1" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>225</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>22</v>
@@ -2981,15 +2984,15 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F2" t="s">
         <v>247</v>
-      </c>
-      <c r="F2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>21</v>
@@ -2998,27 +3001,27 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F3" t="s">
         <v>247</v>
-      </c>
-      <c r="F3" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="15">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>20</v>
@@ -3027,15 +3030,15 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>20</v>
@@ -3044,27 +3047,27 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="15">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>19</v>
@@ -3073,24 +3076,24 @@
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B9" s="4"/>
       <c r="E9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>18</v>
@@ -3099,18 +3102,18 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>17</v>
@@ -3119,18 +3122,18 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>15</v>
@@ -3139,18 +3142,18 @@
         <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>18</v>
@@ -3159,18 +3162,18 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>17</v>
@@ -3179,33 +3182,33 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="15">
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>16</v>
@@ -3214,18 +3217,18 @@
         <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>16</v>
@@ -3234,18 +3237,18 @@
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>16</v>
@@ -3254,18 +3257,18 @@
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>16</v>
@@ -3274,15 +3277,15 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>14</v>
@@ -3291,15 +3294,15 @@
         <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>15</v>
@@ -3308,38 +3311,38 @@
         <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>12</v>
@@ -3348,15 +3351,15 @@
         <v>52</v>
       </c>
       <c r="E24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>9</v>
@@ -3365,15 +3368,15 @@
         <v>54</v>
       </c>
       <c r="E25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>12</v>
@@ -3382,15 +3385,15 @@
         <v>52</v>
       </c>
       <c r="E26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>9</v>
@@ -3399,15 +3402,15 @@
         <v>54</v>
       </c>
       <c r="E27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>11</v>
@@ -3416,15 +3419,15 @@
         <v>56</v>
       </c>
       <c r="E28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>9</v>
@@ -3433,15 +3436,15 @@
         <v>58</v>
       </c>
       <c r="E29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>10</v>
@@ -3450,15 +3453,15 @@
         <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>9</v>
@@ -3467,15 +3470,15 @@
         <v>62</v>
       </c>
       <c r="E31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>8</v>
@@ -3484,27 +3487,27 @@
         <v>66</v>
       </c>
       <c r="E32" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B33" s="4"/>
       <c r="E33" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>8</v>
@@ -3513,15 +3516,15 @@
         <v>66</v>
       </c>
       <c r="E34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F34" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>7</v>
@@ -3530,30 +3533,30 @@
         <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E35" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B36" s="4"/>
       <c r="E36" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F36" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>4</v>
@@ -3562,30 +3565,30 @@
         <v>76</v>
       </c>
       <c r="D37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B38" s="4"/>
       <c r="E38" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F38" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>6</v>
@@ -3594,18 +3597,18 @@
         <v>72</v>
       </c>
       <c r="D39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F39" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>5</v>
@@ -3614,18 +3617,18 @@
         <v>74</v>
       </c>
       <c r="D40" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>3</v>
@@ -3634,18 +3637,18 @@
         <v>78</v>
       </c>
       <c r="D41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E41" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F41" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>3</v>
@@ -3654,30 +3657,30 @@
         <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E42" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F42" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B43" s="4"/>
       <c r="E43" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F43" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>3</v>
@@ -3686,30 +3689,30 @@
         <v>78</v>
       </c>
       <c r="D44" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C47" s="15">
         <v>86</v>
@@ -3717,21 +3720,21 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C48" s="15">
         <v>88</v>
       </c>
       <c r="D48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>2</v>
@@ -3740,17 +3743,22 @@
         <v>92</v>
       </c>
       <c r="D49" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B50" s="2"/>
+        <v>213</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>